<commit_message>
wrapping up final touches
</commit_message>
<xml_diff>
--- a/data/cyber_crimes_overall.xlsx
+++ b/data/cyber_crimes_overall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\NSS\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC9FC59-3ADD-4297-B9CA-3C4CCB1CBA01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B162B06D-9458-4669-A850-7A3220FCE7A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="678" firstSheet="1" activeTab="5" xr2:uid="{83D2063E-A951-4D1F-B1AA-BA3437BDD47B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="678" firstSheet="1" activeTab="5" xr2:uid="{83D2063E-A951-4D1F-B1AA-BA3437BDD47B}"/>
   </bookViews>
   <sheets>
     <sheet name="stats" sheetId="7" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="250">
   <si>
     <t>Age Range</t>
   </si>
@@ -976,9 +976,6 @@
     <t>amout</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>descriptor</t>
   </si>
   <si>
@@ -1028,6 +1025,9 @@
   </si>
   <si>
     <t>social media</t>
+  </si>
+  <si>
+    <t>city</t>
   </si>
 </sst>
 </file>
@@ -9936,21 +9936,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35352629-4D38-4D21-8D38-7B881E7CFAE7}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="90" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="90" t="s">
         <v>231</v>
       </c>
@@ -9958,16 +9959,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="90">
         <v>60000000</v>
       </c>
@@ -9975,16 +9979,19 @@
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E2" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F2" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="90">
         <v>977411</v>
       </c>
@@ -9992,16 +9999,19 @@
         <v>2020</v>
       </c>
       <c r="C3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E3" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="90">
         <v>2000000</v>
       </c>
@@ -10009,16 +10019,19 @@
         <v>2020</v>
       </c>
       <c r="C4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E4" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="90">
         <v>7000000</v>
       </c>
@@ -10026,16 +10039,19 @@
         <v>2020</v>
       </c>
       <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E5" t="s">
         <v>239</v>
       </c>
-      <c r="D5" t="s">
-        <v>240</v>
-      </c>
-      <c r="E5" s="37" t="s">
+      <c r="F5" s="37" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="90">
         <v>190000</v>
       </c>
@@ -10043,16 +10059,19 @@
         <v>2019</v>
       </c>
       <c r="C6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E6" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" t="s">
+        <v>236</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="90">
         <v>866000</v>
       </c>
@@ -10060,16 +10079,19 @@
         <v>2019</v>
       </c>
       <c r="C7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
-      </c>
-      <c r="E7" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>236</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="90">
         <v>138000</v>
       </c>
@@ -10077,16 +10099,19 @@
         <v>2019</v>
       </c>
       <c r="C8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>237</v>
-      </c>
-      <c r="E8" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="90">
         <v>3000000</v>
       </c>
@@ -10094,16 +10119,19 @@
         <v>2019</v>
       </c>
       <c r="C9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D9" t="s">
-        <v>240</v>
-      </c>
-      <c r="E9" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="90">
         <v>50000</v>
       </c>
@@ -10114,13 +10142,16 @@
         <v>158</v>
       </c>
       <c r="D10" t="s">
-        <v>237</v>
-      </c>
-      <c r="E10" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="90">
         <v>54000</v>
       </c>
@@ -10128,16 +10159,19 @@
         <v>2018</v>
       </c>
       <c r="C11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D11" t="s">
-        <v>237</v>
-      </c>
-      <c r="E11" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" t="s">
+        <v>236</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="90">
         <v>1000000</v>
       </c>
@@ -10145,16 +10179,19 @@
         <v>2018</v>
       </c>
       <c r="C12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D12" t="s">
-        <v>237</v>
-      </c>
-      <c r="E12" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="90">
         <v>50000</v>
       </c>
@@ -10165,13 +10202,16 @@
         <v>158</v>
       </c>
       <c r="D13" t="s">
-        <v>237</v>
-      </c>
-      <c r="E13" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13" t="s">
+        <v>236</v>
+      </c>
+      <c r="F13" s="37" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="90">
         <v>388000</v>
       </c>
@@ -10179,16 +10219,19 @@
         <v>2018</v>
       </c>
       <c r="C14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D14" t="s">
-        <v>237</v>
-      </c>
-      <c r="E14" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="37" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="90">
         <v>200000</v>
       </c>
@@ -10196,16 +10239,19 @@
         <v>2017</v>
       </c>
       <c r="C15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D15" t="s">
-        <v>237</v>
-      </c>
-      <c r="E15" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" t="s">
+        <v>236</v>
+      </c>
+      <c r="F15" s="37" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="90">
         <v>25000</v>
       </c>
@@ -10213,16 +10259,19 @@
         <v>2017</v>
       </c>
       <c r="C16" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="s">
         <v>248</v>
       </c>
-      <c r="D16" t="s">
-        <v>249</v>
-      </c>
-      <c r="E16" s="37" t="s">
+      <c r="F16" s="37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="90">
         <v>232258</v>
       </c>
@@ -10230,16 +10279,19 @@
         <v>2016</v>
       </c>
       <c r="C17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D17" t="s">
-        <v>237</v>
-      </c>
-      <c r="E17" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="90">
         <v>279277</v>
       </c>
@@ -10247,12 +10299,15 @@
         <v>2016</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" t="s">
-        <v>237</v>
-      </c>
-      <c r="E18" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" t="s">
+        <v>236</v>
+      </c>
+      <c r="F18" s="37" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>